<commit_message>
Supp tables for MH and contrasting all periods
</commit_message>
<xml_diff>
--- a/Supplmentary_Maize_Period_Contrasts.xlsx
+++ b/Supplmentary_Maize_Period_Contrasts.xlsx
@@ -1,23 +1,82 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/185965a385c69db2/Documents/Moquegua_Morphology/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_BB720C9D2FB5A8FECA5755B24730BC45D27E9374" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7E45350-58E0-4BF4-836D-B80CB3E7BDCA}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LF_vs_MH" sheetId="1" r:id="rId1"/>
     <sheet name="Within_MH" sheetId="2" r:id="rId2"/>
     <sheet name="LIP_vs_Others" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
+  <si>
+    <t>contrast</t>
+  </si>
+  <si>
+    <t>estimate</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>t.ratio</t>
+  </si>
+  <si>
+    <t>p.value</t>
+  </si>
+  <si>
+    <t>(LF/MH) - LF</t>
+  </si>
+  <si>
+    <t>LIP - LF</t>
+  </si>
+  <si>
+    <t>MH - LF</t>
+  </si>
+  <si>
+    <t>LF - (LF/MH)</t>
+  </si>
+  <si>
+    <t>LF - LIP</t>
+  </si>
+  <si>
+    <t>LF - MH</t>
+  </si>
+  <si>
+    <t>(LF/MH) - LIP</t>
+  </si>
+  <si>
+    <t>(LF/MH) - MH</t>
+  </si>
+  <si>
+    <t>LIP - MH</t>
+  </si>
+  <si>
+    <t>MH - LIP</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -61,17 +120,25 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -109,7 +176,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -143,6 +210,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -177,9 +245,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -352,50 +421,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>contrast</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>estimate</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>SE</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>df</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>t.ratio</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>p.value</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>(LF/MH) - LF</t>
-        </is>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>6</v>
       </c>
       <c r="B2">
         <v>-0.1164308474943561</v>
@@ -407,20 +462,18 @@
         <v>340</v>
       </c>
       <c r="E2">
-        <v>-0.06895532306930639</v>
+        <v>-6.8955323069306393E-2</v>
       </c>
       <c r="F2">
-        <v>0.9981994074641909</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>LIP - LF</t>
-        </is>
+        <v>0.99819940746419089</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>-6.401177117298401</v>
+        <v>-6.4011771172984009</v>
       </c>
       <c r="C3">
         <v>1.656535053108616</v>
@@ -429,20 +482,18 @@
         <v>340</v>
       </c>
       <c r="E3">
-        <v>-3.864196598367236</v>
+        <v>-3.8641965983672359</v>
       </c>
       <c r="F3">
-        <v>0.0003945627614647673</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>MH - LF</t>
-        </is>
+        <v>3.9456276146476732E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>-3.434259414443965</v>
+        <v>-3.4342594144439649</v>
       </c>
       <c r="C4">
         <v>1.15018140488151</v>
@@ -451,10 +502,10 @@
         <v>340</v>
       </c>
       <c r="E4">
-        <v>-2.985841537577073</v>
+        <v>-2.9858415375770728</v>
       </c>
       <c r="F4">
-        <v>0.008692080133153479</v>
+        <v>8.6920801331534792E-3</v>
       </c>
     </row>
   </sheetData>
@@ -463,50 +514,39 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.1796875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>contrast</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>estimate</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>SE</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>df</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>t.ratio</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>p.value</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>LF - (LF/MH)</t>
-        </is>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>9</v>
       </c>
       <c r="B2">
         <v>0.1164308474943561</v>
@@ -518,20 +558,18 @@
         <v>340</v>
       </c>
       <c r="E2">
-        <v>0.06895532306930639</v>
+        <v>6.8955323069306393E-2</v>
       </c>
       <c r="F2">
-        <v>0.9450657173534409</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>LF - LIP</t>
-        </is>
+        <v>0.94506571735344092</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>10</v>
       </c>
       <c r="B3">
-        <v>6.401177117298401</v>
+        <v>6.4011771172984009</v>
       </c>
       <c r="C3">
         <v>1.656535053108616</v>
@@ -540,20 +578,18 @@
         <v>340</v>
       </c>
       <c r="E3">
-        <v>3.864196598367236</v>
+        <v>3.8641965983672359</v>
       </c>
       <c r="F3">
-        <v>0.0008008704171354587</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>LF - MH</t>
-        </is>
+        <v>8.0087041713545874E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>11</v>
       </c>
       <c r="B4">
-        <v>3.434259414443965</v>
+        <v>3.4342594144439649</v>
       </c>
       <c r="C4">
         <v>1.15018140488151</v>
@@ -562,39 +598,35 @@
         <v>340</v>
       </c>
       <c r="E4">
-        <v>2.985841537577073</v>
+        <v>2.9858415375770728</v>
       </c>
       <c r="F4">
-        <v>0.006066150452353481</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>(LF/MH) - LIP</t>
-        </is>
+        <v>6.0661504523534812E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>12</v>
       </c>
       <c r="B5">
         <v>6.284746269804045</v>
       </c>
       <c r="C5">
-        <v>1.760819722217095</v>
+        <v>1.7608197222170949</v>
       </c>
       <c r="D5">
         <v>340</v>
       </c>
       <c r="E5">
-        <v>3.569216195449443</v>
+        <v>3.5692161954494428</v>
       </c>
       <c r="F5">
-        <v>0.001228644648969924</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>(LF/MH) - MH</t>
-        </is>
+        <v>1.2286446489699239E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>13</v>
       </c>
       <c r="B6">
         <v>3.317828566949609</v>
@@ -606,17 +638,15 @@
         <v>340</v>
       </c>
       <c r="E6">
-        <v>2.560297592280702</v>
+        <v>2.5602975922807021</v>
       </c>
       <c r="F6">
-        <v>0.01633474167277283</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>LIP - MH</t>
-        </is>
+        <v>1.633474167277283E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>14</v>
       </c>
       <c r="B7">
         <v>-2.966917702854436</v>
@@ -628,10 +658,10 @@
         <v>340</v>
       </c>
       <c r="E7">
-        <v>-2.366064147091207</v>
+        <v>-2.3660641470912069</v>
       </c>
       <c r="F7">
-        <v>0.02224634627607847</v>
+        <v>2.2246346276078469E-2</v>
       </c>
     </row>
   </sheetData>
@@ -640,53 +670,39 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>contrast</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>estimate</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>SE</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>df</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>t.ratio</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>p.value</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>LF - LIP</t>
-        </is>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>10</v>
       </c>
       <c r="B2">
-        <v>6.401177117298401</v>
+        <v>6.4011771172984009</v>
       </c>
       <c r="C2">
         <v>1.656535053108616</v>
@@ -695,39 +711,35 @@
         <v>340</v>
       </c>
       <c r="E2">
-        <v>3.864196598367236</v>
+        <v>3.8641965983672359</v>
       </c>
       <c r="F2">
-        <v>0.0003945627614647673</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>(LF/MH) - LIP</t>
-        </is>
+        <v>3.9456276146476732E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>12</v>
       </c>
       <c r="B3">
         <v>6.284746269804045</v>
       </c>
       <c r="C3">
-        <v>1.760819722217095</v>
+        <v>1.7608197222170949</v>
       </c>
       <c r="D3">
         <v>340</v>
       </c>
       <c r="E3">
-        <v>3.569216195449443</v>
+        <v>3.5692161954494428</v>
       </c>
       <c r="F3">
-        <v>0.001202026371455389</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>MH - LIP</t>
-        </is>
+        <v>1.2020263714553889E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>15</v>
       </c>
       <c r="B4">
         <v>2.966917702854436</v>
@@ -739,10 +751,10 @@
         <v>340</v>
       </c>
       <c r="E4">
-        <v>2.366064147091207</v>
+        <v>2.3660641470912069</v>
       </c>
       <c r="F4">
-        <v>0.05054044867030072</v>
+        <v>5.0540448670300719E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>